<commit_message>
metricas incluidad a netmhcpan4.1
</commit_message>
<xml_diff>
--- a/metrics/metrics.xlsx
+++ b/metrics/metrics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Models</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>protbert_bfd_freeze</t>
+  </si>
+  <si>
+    <t>netMHCpan4.1</t>
+  </si>
+  <si>
+    <t>netMHCpan4.1 (no WB)</t>
+  </si>
+  <si>
+    <t>sin considerar el WB</t>
   </si>
 </sst>
 </file>
@@ -61,10 +70,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -85,7 +94,21 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -99,8 +122,107 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -113,121 +235,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,43 +257,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,139 +431,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,11 +472,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,11 +502,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -510,47 +561,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -559,152 +574,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -730,6 +745,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1051,15 +1075,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75" outlineLevelRow="7" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="15.4814814814815" customWidth="1"/>
+    <col min="1" max="1" width="18.8148148148148" customWidth="1"/>
     <col min="2" max="6" width="12.4444444444444" style="1"/>
   </cols>
   <sheetData>
@@ -1223,6 +1247,49 @@
         <v>0.908303395526712</v>
       </c>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.900557292917419</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.95855328768034</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.837161769829288</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.893754455568298</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.900689535287982</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.830918695507239</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.984410329644174</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.672442225060968</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.799056102559148</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.831249275698226</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
metricas comparativas con 30 epochs
</commit_message>
<xml_diff>
--- a/metrics/metrics.xlsx
+++ b/metrics/metrics.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Model</t>
   </si>
@@ -126,6 +126,51 @@
   </si>
   <si>
     <t>Luego baja el desempeño en training para mas epochs</t>
+  </si>
+  <si>
+    <t>esm2_t30_30_epochs</t>
+  </si>
+  <si>
+    <t>Freeze es mejor. Acc_steps permite entrenar modelos grandes, pero toma mas epochs y no llega a superar al modelo sin acc_steps.</t>
+  </si>
+  <si>
+    <t>esm2_t30_acc_steps_30_epochs</t>
+  </si>
+  <si>
+    <t>17 epochs</t>
+  </si>
+  <si>
+    <t>esm2_t30_freeze_30_epochs</t>
+  </si>
+  <si>
+    <t>14 epochs</t>
+  </si>
+  <si>
+    <t>esm2_t30_freeze_acc_steps_30_epochs</t>
+  </si>
+  <si>
+    <t>27 epochs</t>
+  </si>
+  <si>
+    <t>esm2_t6_30_epochs</t>
+  </si>
+  <si>
+    <t>9 epochs</t>
+  </si>
+  <si>
+    <t>esm2_t6_acc_steps_30_epochs</t>
+  </si>
+  <si>
+    <t>15 epochs</t>
+  </si>
+  <si>
+    <t>esm2_t6_freeze_30_epochs</t>
+  </si>
+  <si>
+    <t>6 epochs</t>
+  </si>
+  <si>
+    <t>esm2_t6_freeze_acc_steps_30_epochs</t>
   </si>
   <si>
     <t>tape 30 epochs</t>
@@ -139,11 +184,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.0000_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -177,30 +222,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,7 +239,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,16 +291,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,7 +337,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,37 +357,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -340,108 +385,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -454,36 +553,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -496,31 +565,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,7 +678,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,6 +687,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -662,17 +718,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -692,6 +748,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -700,173 +771,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -876,132 +921,150 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1403,56 +1466,57 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88666666666667" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88666666666667" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="22.9933333333333" customWidth="1"/>
-    <col min="2" max="2" width="11.3733333333333" style="1" customWidth="1"/>
-    <col min="3" max="6" width="12.4466666666667" style="1"/>
+    <col min="1" max="1" width="30.8666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3733333333333" style="2" customWidth="1"/>
+    <col min="3" max="6" width="12.4466666666667" style="2"/>
+    <col min="8" max="8" width="24.9333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:6">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>0.5</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>0.498957005</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>0.665738915</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="35">
         <v>0.498957005</v>
       </c>
       <c r="G2" t="s">
@@ -1460,445 +1524,445 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="36"/>
       <c r="G3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="11">
         <v>0.934549339204924</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="11">
         <v>0.928260670452463</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="12">
         <v>0.941563116943444</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="11">
         <v>0.9348</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="37">
         <v>0.934534708540966</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:6">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="32"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>0.934449719032475</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="14">
         <v>0.933389730337339</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="13">
         <v>0.935373359656253</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="13">
         <v>0.934380492218812</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="38">
         <v>0.934447792328195</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>0.898625202269851</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>0.896612716763005</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <v>0.900673557078155</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <v>0.898638549330861</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="36">
         <v>0.898620929424035</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="15">
         <v>0.935125993702037</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="11">
         <v>0.925277046053229</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="15">
         <v>0.946359307862036</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="15">
         <v>0.93569944081478</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="39">
         <v>0.935102561131069</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:6">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="11">
         <v>0.886862649438484</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="11">
         <v>0.891342932706435</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="11">
         <v>0.880629427476483</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="11">
         <v>0.885953792680433</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="37">
         <v>0.886875651871595</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="16">
         <v>0.932694557888571</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="16">
         <v>0.924319582578579</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="13">
         <v>0.942213447915457</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="16">
         <v>0.933180743816386</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="40">
         <v>0.932674701587669</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="17">
         <v>0.900982495582117</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="17">
         <v>0.927920556402722</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="17">
         <v>0.869202183253977</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="17">
         <v>0.89760210108472</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="41">
         <v>0.901048788967435</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="12">
         <v>0.934441137836383</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="12">
         <v>0.925051147988179</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="12">
         <v>0.945139937289513</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="12">
         <v>0.934987650066057</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="42">
         <v>0.934418820257272</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:6">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="19">
         <v>0.880567617884542</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="19">
         <v>0.855600686374595</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="19">
         <v>0.91489954709093</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="19">
         <v>0.884257076795294</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="43">
         <v>0.880496001854212</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="20">
         <v>0.5</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="20">
         <v>0.498957005446749</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="20">
         <v>1</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="20">
         <v>0.665738915304031</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="44">
         <v>0.498957005446749</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="17">
         <v>0.908949606669102</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="17">
         <v>0.91668639613618</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="17">
         <v>0.899291603762629</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="17">
         <v>0.907905689798693</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="41">
         <v>0.908969753157955</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="12">
         <v>0.930287088182664</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="12">
         <v>0.918468804374844</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
         <v>0.944025084194634</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="12">
         <v>0.931071608558207</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="42">
         <v>0.930258430872638</v>
       </c>
     </row>
-    <row r="17" ht="15.75" spans="1:6">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="37"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>0.5</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>0.498957005</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <v>1</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6">
         <v>0.665738915</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="35">
         <v>0.498957005</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="20">
         <v>0.500011564704521</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="20">
         <v>0.49896278784086</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="20">
         <v>1</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="20">
         <v>0.665744062345373</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="44">
         <v>0.498968594275118</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="12">
         <v>0.681609741330289</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="12">
         <v>0.713917313653946</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="12">
         <v>0.604412960167228</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="12">
         <v>0.65461726159032</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="42">
         <v>0.681770772974852</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="1:6">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="38"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="20">
         <v>0.5</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="20">
         <v>0.498957005446749</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="20">
         <v>1</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="20">
         <v>0.665738915304031</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="44">
         <v>0.498957005446749</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="39"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="44"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="12">
         <v>0.908279462864264</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="12">
         <v>0.917552843886268</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="12">
         <v>0.896806410405295</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="12">
         <v>0.907061013783747</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="42">
         <v>0.908303395526712</v>
       </c>
     </row>
-    <row r="25" ht="15.75" spans="1:6">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:6">
+      <c r="A25" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="38"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="22">
         <v>0.900557292917419</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="23">
         <v>0.95855328768034</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="22">
         <v>0.837161769829288</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="22">
         <v>0.893754455568298</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="45">
         <v>0.900689535287982</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="1:7">
-      <c r="A27" s="23" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="25">
         <v>0.830918695507239</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="26">
         <v>0.984410329644174</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="25">
         <v>0.672442225060968</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="25">
         <v>0.799056102559148</v>
       </c>
-      <c r="F27" s="41">
+      <c r="F27" s="46">
         <v>0.831249275698226</v>
       </c>
       <c r="G27" t="s">
@@ -1906,45 +1970,226 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="28">
         <v>0.93930203590237</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="29">
         <v>0.944656735370542</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="30">
         <v>0.933039135988851</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="28">
         <v>0.938811995723324</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="28">
         <v>0.939315100243365</v>
       </c>
       <c r="G29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
+    <row r="32" spans="1:8">
+      <c r="A32" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="C32" s="32">
+        <v>0.498957005446749</v>
+      </c>
+      <c r="D32" s="32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="32">
+        <v>0.665738915304031</v>
+      </c>
+      <c r="F32" s="32">
+        <v>0.498957005446749</v>
+      </c>
+      <c r="H32" s="47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.934570882512929</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0.933727536231884</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.935245616072465</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.934485959619401</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.934569475026074</v>
+      </c>
+      <c r="G33" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="33">
+        <v>0.939272274012397</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0.930368077211991</v>
+      </c>
+      <c r="D34" s="34">
+        <v>0.949297410289165</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0.939737429011565</v>
+      </c>
+      <c r="F34" s="33">
+        <v>0.939251361687333</v>
+      </c>
+      <c r="G34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="47"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="12">
+        <v>0.93630037662043</v>
+      </c>
+      <c r="C35" s="12">
+        <v>0.93190887450119</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0.941075368714435</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.936469690928946</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0.936290416038938</v>
+      </c>
+      <c r="G35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" s="47"/>
+    </row>
+    <row r="36" spans="8:8">
+      <c r="H36" s="47"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="12">
+        <v>0.938980598626764</v>
+      </c>
+      <c r="C37" s="12">
+        <v>0.933250020063975</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0.945290906979444</v>
+      </c>
+      <c r="E37" s="12">
+        <v>0.93923187427523</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.938967435392281</v>
+      </c>
+      <c r="G37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="47"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="12">
+        <v>0.936590001893248</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0.932236138425973</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0.941319242828939</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0.936755672920795</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0.936580136748174</v>
+      </c>
+      <c r="G38" t="s">
+        <v>48</v>
+      </c>
+      <c r="H38" s="47"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="34">
+        <v>0.940109036992643</v>
+      </c>
+      <c r="C39" s="34">
+        <v>0.939830508474576</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0.940157937521774</v>
+      </c>
+      <c r="E39" s="34">
+        <v>0.93999419448476</v>
+      </c>
+      <c r="F39" s="34">
+        <v>0.940108934986672</v>
+      </c>
+      <c r="G39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="47"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="12">
+        <v>0.935398406891108</v>
+      </c>
+      <c r="C40" s="12">
+        <v>0.932594644506001</v>
+      </c>
+      <c r="D40" s="12">
+        <v>0.938334688189525</v>
+      </c>
+      <c r="E40" s="12">
+        <v>0.935455861070911</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0.935392281840306</v>
+      </c>
+      <c r="G40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="47"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H32:H40"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1963,10 +2208,10 @@
   <sheetData>
     <row r="2" spans="4:13">
       <c r="D2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>